<commit_message>
docs: se cambia la lista netdecked
</commit_message>
<xml_diff>
--- a/data/netdecked.xlsx
+++ b/data/netdecked.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuar\Desktop\CA0305\Proyecto_individual\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuar\Desktop\CA0305\Proyecto_individual\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="36">
   <si>
     <t>Carta</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Defensive</t>
   </si>
   <si>
-    <t>Rescue-ACE Hydrant</t>
-  </si>
-  <si>
     <t>Starter</t>
   </si>
   <si>
@@ -56,30 +53,15 @@
     <t>Ash Blossom &amp; Joyous Spring</t>
   </si>
   <si>
-    <t>Rescue-ACE Impulse</t>
-  </si>
-  <si>
-    <t>Rescue-ACE Air Lifter</t>
-  </si>
-  <si>
-    <t>Rescue-ACE Fire Engine</t>
-  </si>
-  <si>
     <t>Garnet</t>
   </si>
   <si>
     <t>Diabellstar the Black Witch</t>
   </si>
   <si>
-    <t>Rescue-ACE Preventer</t>
-  </si>
-  <si>
     <t>Combo piece</t>
   </si>
   <si>
-    <t>Rescue-ACE Turbulence</t>
-  </si>
-  <si>
     <t>Bonfire</t>
   </si>
   <si>
@@ -92,22 +74,64 @@
     <t>Called by the Grave</t>
   </si>
   <si>
-    <t>RESCUE!</t>
-  </si>
-  <si>
-    <t>ALERT!</t>
-  </si>
-  <si>
-    <t>EMERGENCY!</t>
-  </si>
-  <si>
     <t>WANTED: Seeket of Sinful Spoils</t>
   </si>
   <si>
-    <t>CONTAIN!</t>
-  </si>
-  <si>
-    <t>EXTINGUISH!</t>
+    <t>Fire King High Avatar Kirin</t>
+  </si>
+  <si>
+    <t>Legendary Fire King Ponix</t>
+  </si>
+  <si>
+    <t>Sacred Fire King Garunix</t>
+  </si>
+  <si>
+    <t>Fire King Island</t>
+  </si>
+  <si>
+    <t>Fire King Sanctuary</t>
+  </si>
+  <si>
+    <t>Fire King Avatar Arvata</t>
+  </si>
+  <si>
+    <t>Snake-Eye Ash</t>
+  </si>
+  <si>
+    <t>Snake-Eyes Flamberge Dragon</t>
+  </si>
+  <si>
+    <t>Fire King Sky Burn</t>
+  </si>
+  <si>
+    <t>Infinite Impermanence</t>
+  </si>
+  <si>
+    <t>Nibiru the Primal Being</t>
+  </si>
+  <si>
+    <t>Snake-Eye Oak</t>
+  </si>
+  <si>
+    <t>Fire King Courtier Ulcanix</t>
+  </si>
+  <si>
+    <t>Non engine</t>
+  </si>
+  <si>
+    <t>One for one</t>
+  </si>
+  <si>
+    <t>Sinful Spoils of Subversion - Snake-Eye</t>
+  </si>
+  <si>
+    <t>Divine Temple of the Snale-Eye</t>
+  </si>
+  <si>
+    <t>Triple Tactic Talent</t>
+  </si>
+  <si>
+    <t>Crossout Designator</t>
   </si>
 </sst>
 </file>
@@ -425,13 +449,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -449,10 +475,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -460,76 +486,76 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -537,54 +563,54 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -592,32 +618,32 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -625,21 +651,21 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C18">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -650,20 +676,97 @@
         <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>27</v>
       </c>
-      <c r="B21" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21">
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
docs: se arregla un error de digitacion
</commit_message>
<xml_diff>
--- a/data/netdecked.xlsx
+++ b/data/netdecked.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
   <si>
     <t>Carta</t>
   </si>
@@ -116,19 +116,10 @@
     <t>Fire King Courtier Ulcanix</t>
   </si>
   <si>
-    <t>Non engine</t>
-  </si>
-  <si>
     <t>One for one</t>
   </si>
   <si>
-    <t>Sinful Spoils of Subversion - Snake-Eye</t>
-  </si>
-  <si>
     <t>Divine Temple of the Snale-Eye</t>
-  </si>
-  <si>
-    <t>Triple Tactic Talent</t>
   </si>
   <si>
     <t>Crossout Designator</t>
@@ -449,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,7 +505,7 @@
         <v>5</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -662,7 +653,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B19" t="s">
         <v>4</v>
@@ -723,15 +714,15 @@
         <v>5</v>
       </c>
       <c r="C24">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -742,31 +733,9 @@
         <v>31</v>
       </c>
       <c r="B26" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>33</v>
-      </c>
-      <c r="B28" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28">
         <v>1</v>
       </c>
     </row>

</xml_diff>